<commit_message>
Added new year and location metadata for South Australian Museum samples which were missing metadata previously.
</commit_message>
<xml_diff>
--- a/PCA-metadata.xlsx
+++ b/PCA-metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="460" windowWidth="27140" windowHeight="15980" tabRatio="500"/>
+    <workbookView xWindow="660" yWindow="700" windowWidth="27140" windowHeight="15980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="PCA" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="402">
   <si>
     <t>WAM63_R1.fastq.gz</t>
   </si>
@@ -1370,7 +1370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1465,6 +1465,9 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1744,8 +1747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="G124" sqref="G124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1870,7 +1873,7 @@
         <v>2005</v>
       </c>
       <c r="L2" s="18">
-        <f t="shared" ref="L2:L19" si="0">2019-K2</f>
+        <f t="shared" ref="L2:L20" si="0">2019-K2</f>
         <v>14</v>
       </c>
       <c r="M2" s="3">
@@ -2246,9 +2249,15 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="37"/>
+      <c r="M7" s="29">
+        <v>-26.578333000000001</v>
+      </c>
+      <c r="N7" s="29">
+        <v>136.96111110000001</v>
+      </c>
+      <c r="O7" s="37" t="s">
+        <v>391</v>
+      </c>
       <c r="P7" s="38">
         <v>0.169769</v>
       </c>
@@ -3188,12 +3197,19 @@
       <c r="H20" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="I20" s="40"/>
+      <c r="I20" s="46">
+        <v>38403</v>
+      </c>
       <c r="J20" s="34" t="s">
         <v>385</v>
       </c>
-      <c r="K20" s="35"/>
-      <c r="L20" s="36"/>
+      <c r="K20" s="35">
+        <v>2005</v>
+      </c>
+      <c r="L20" s="36">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
       <c r="M20" s="29">
         <v>-27.4086</v>
       </c>
@@ -3269,8 +3285,12 @@
         <f t="shared" ref="L21:L52" si="1">2019-K21</f>
         <v>22</v>
       </c>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
+      <c r="M21" s="29">
+        <v>-32.19</v>
+      </c>
+      <c r="N21" s="29">
+        <v>138.012</v>
+      </c>
       <c r="O21" s="39" t="s">
         <v>391</v>
       </c>
@@ -4852,9 +4872,15 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="O42" s="37"/>
+      <c r="M42" s="29">
+        <v>-26.577999999999999</v>
+      </c>
+      <c r="N42" s="29">
+        <v>137.09299999999999</v>
+      </c>
+      <c r="O42" s="37" t="s">
+        <v>391</v>
+      </c>
       <c r="P42" s="38">
         <v>0.189141</v>
       </c>
@@ -8086,7 +8112,7 @@
         <v>2009</v>
       </c>
       <c r="L85" s="18">
-        <f t="shared" ref="L85:L116" si="3">2019-K85</f>
+        <f t="shared" ref="L85" si="3">2019-K85</f>
         <v>10</v>
       </c>
       <c r="M85" s="5">
@@ -9744,8 +9770,12 @@
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="M107" s="29"/>
-      <c r="N107" s="29"/>
+      <c r="M107" s="29">
+        <v>-32.521999999999998</v>
+      </c>
+      <c r="N107" s="29">
+        <v>135.322</v>
+      </c>
       <c r="O107" s="39" t="s">
         <v>391</v>
       </c>

</xml_diff>